<commit_message>
added copies of actions in order to run natively from UFT instead of just from MBT
</commit_message>
<xml_diff>
--- a/DCM2_VacationRequest/Default.xlsx
+++ b/DCM2_VacationRequest/Default.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,10 @@
     <sheet name="DCM2_Logout_UFT_AI" sheetId="4" r:id="rId4"/>
     <sheet name="DCM2_ApproveRequest_UFT_AI" sheetId="5" r:id="rId5"/>
     <sheet name="DCM2_ViewApproval_UFT_AI" sheetId="6" r:id="rId6"/>
+    <sheet name="Copy of DCM2_Login_UFT_AI" sheetId="7" r:id="rId7"/>
+    <sheet name="Copy of DCM2_Logout_UFT_AI" sheetId="8" r:id="rId8"/>
+    <sheet name="Copy 2 of DCM2_Login_UFT_AI" sheetId="9" r:id="rId9"/>
+    <sheet name="Copy 2 of DCM2_Logout_UFT_AI" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -488,6 +492,25 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
@@ -568,7 +591,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -581,4 +604,61 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.95"/>
+  <cols>
+    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.95"/>
+  <cols>
+    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added unit for denying the vacation request
</commit_message>
<xml_diff>
--- a/DCM2_VacationRequest/Default.xlsx
+++ b/DCM2_VacationRequest/Default.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="9"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Copy of DCM2_Logout_UFT_AI" sheetId="8" r:id="rId8"/>
     <sheet name="Copy 2 of DCM2_Login_UFT_AI" sheetId="9" r:id="rId9"/>
     <sheet name="Copy 2 of DCM2_Logout_UFT_AI" sheetId="10" r:id="rId10"/>
+    <sheet name="DCM2_DenyRequest_UFT_AI" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -191,10 +192,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="FFFFFF"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="283845"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -481,9 +482,66 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1"/>
@@ -492,11 +550,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -511,7 +569,64 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -530,7 +645,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -549,64 +664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
-  <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="14.95" customFormat="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
-  <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="14.95" customFormat="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
-  <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="14.95" customFormat="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -623,42 +681,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
-  <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="14.95" customFormat="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
-  <cols>
-    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>